<commit_message>
Filters Works successfully, Logs Added, I'm tired
Co-Authored-By: Evgeniy Sapov <32373244+BubbaCat@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/bin/Debug/PetRegistry.xlsx
+++ b/bin/Debug/PetRegistry.xlsx
@@ -5,38 +5,95 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\м видео\Desktop\прежде чем ты начнешь\5 сем\пис\PetRegistry\bin\Debug\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sergey\Documents\GitHub\PetRegistry\bin\Debug\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DA6016E8-D493-4ABF-83D2-CD8018C78888}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CFA47DD0-444E-490C-8F48-5EBA632278D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10812" yWindow="2580" windowWidth="12228" windowHeight="8496" xr2:uid="{06A27F28-C0DA-400C-BFE1-5ADE42EC4CAD}"/>
+    <workbookView xWindow="5760" yWindow="3396" windowWidth="17280" windowHeight="8964" xr2:uid="{68133A1F-89D3-414D-8F13-2970D7B57E53}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>y</t>
-  </si>
-  <si>
-    <t>r</t>
-  </si>
-  <si>
-    <t>h</t>
-  </si>
-  <si>
-    <t>e</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="20">
+  <si>
+    <t>Кошка</t>
+  </si>
+  <si>
+    <t>Женский</t>
+  </si>
+  <si>
+    <t>19.09.2019</t>
+  </si>
+  <si>
+    <t>Вася</t>
+  </si>
+  <si>
+    <t>Sapov EV</t>
+  </si>
+  <si>
+    <t>Собака</t>
+  </si>
+  <si>
+    <t>Тося</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Ромашка</t>
+  </si>
+  <si>
+    <t>Мужской</t>
+  </si>
+  <si>
+    <t>Бося</t>
+  </si>
+  <si>
+    <t>Жося</t>
+  </si>
+  <si>
+    <t>Гусь</t>
+  </si>
+  <si>
+    <t>Цветок</t>
+  </si>
+  <si>
+    <t>Дося</t>
+  </si>
+  <si>
+    <t>Lap YD</t>
+  </si>
+  <si>
+    <t>04.06.2020</t>
+  </si>
+  <si>
+    <t>Жук</t>
+  </si>
+  <si>
+    <t>01.12.2021</t>
+  </si>
+  <si>
+    <t>Зая</t>
   </si>
 </sst>
 </file>
@@ -388,8 +445,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A5955F7-778F-49F6-909B-35AE655BEB76}">
-  <dimension ref="A2:I2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DAC3DF7-993F-4EC5-BDB7-B3E6620E5CBB}">
+  <dimension ref="A2:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -397,7 +454,7 @@
   <sheetData>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -409,19 +466,213 @@
         <v>2</v>
       </c>
       <c r="E2">
+        <v>123</v>
+      </c>
+      <c r="F2">
+        <v>123</v>
+      </c>
+      <c r="G2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>123</v>
+      </c>
+      <c r="F3">
+        <v>123</v>
+      </c>
+      <c r="G3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" t="s">
         <v>8</v>
       </c>
-      <c r="F2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G2">
-        <v>6</v>
-      </c>
-      <c r="H2">
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
         <v>2</v>
       </c>
-      <c r="I2">
+      <c r="E4">
+        <v>123</v>
+      </c>
+      <c r="F4">
+        <v>123</v>
+      </c>
+      <c r="G4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I4" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>1002</v>
+      </c>
+      <c r="B5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5">
+        <v>123</v>
+      </c>
+      <c r="F5">
+        <v>123</v>
+      </c>
+      <c r="G5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" t="s">
+        <v>7</v>
+      </c>
+      <c r="I5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>1003</v>
+      </c>
+      <c r="B6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6">
+        <v>123</v>
+      </c>
+      <c r="F6">
+        <v>123</v>
+      </c>
+      <c r="G6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" t="s">
+        <v>7</v>
+      </c>
+      <c r="I6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>1004</v>
+      </c>
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7">
+        <v>123</v>
+      </c>
+      <c r="F7">
+        <v>123</v>
+      </c>
+      <c r="G7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>2002</v>
+      </c>
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8">
+        <v>123</v>
+      </c>
+      <c r="F8">
+        <v>123</v>
+      </c>
+      <c r="G8" t="s">
+        <v>17</v>
+      </c>
+      <c r="I8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>2007</v>
+      </c>
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9" t="s">
+        <v>19</v>
+      </c>
+      <c r="I9" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added headers in export file
Co-Authored-By: Evgeniy Sapov <32373244+BubbaCat@users.noreply.github.com>
Co-Authored-By: Anastasia <83288552+puzyreevskaya@users.noreply.github.com>
Co-Authored-By: Sergey Zhenikhov <84619957+zhenihovs@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/bin/Debug/PetRegistry.xlsx
+++ b/bin/Debug/PetRegistry.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sergey\Documents\GitHub\PetRegistry\bin\Debug\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ПИС\PetRegistry\bin\Debug\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CFA47DD0-444E-490C-8F48-5EBA632278D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A0B99D67-A9E9-4519-AC01-37068CDAB84F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="3396" windowWidth="17280" windowHeight="8964" xr2:uid="{68133A1F-89D3-414D-8F13-2970D7B57E53}"/>
+    <workbookView xWindow="4965" yWindow="3315" windowWidth="21480" windowHeight="11865" xr2:uid="{5CA92843-8467-4E82-A10C-44E403B9B0B8}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -34,41 +34,68 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="29">
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Категория</t>
+  </si>
+  <si>
+    <t>Пол</t>
+  </si>
+  <si>
+    <t>Дата рождения</t>
+  </si>
+  <si>
+    <t>Идентификационная метка</t>
+  </si>
+  <si>
+    <t>Номер электронного чипа</t>
+  </si>
+  <si>
+    <t>Кличка</t>
+  </si>
+  <si>
+    <t>Фото</t>
+  </si>
+  <si>
+    <t>Владелец</t>
+  </si>
+  <si>
+    <t>Собака</t>
+  </si>
+  <si>
+    <t>Мужской</t>
+  </si>
+  <si>
+    <t>19.09.2019</t>
+  </si>
+  <si>
+    <t>Вася</t>
+  </si>
+  <si>
+    <t>Sapov EV</t>
+  </si>
+  <si>
+    <t>Женский</t>
+  </si>
+  <si>
+    <t>Тося</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Ромашка</t>
+  </si>
+  <si>
+    <t>Бося</t>
+  </si>
   <si>
     <t>Кошка</t>
   </si>
   <si>
-    <t>Женский</t>
-  </si>
-  <si>
-    <t>19.09.2019</t>
-  </si>
-  <si>
-    <t>Вася</t>
-  </si>
-  <si>
-    <t>Sapov EV</t>
-  </si>
-  <si>
-    <t>Собака</t>
-  </si>
-  <si>
-    <t>Тося</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>Ромашка</t>
-  </si>
-  <si>
-    <t>Мужской</t>
-  </si>
-  <si>
-    <t>Бося</t>
-  </si>
-  <si>
     <t>Жося</t>
   </si>
   <si>
@@ -84,16 +111,16 @@
     <t>Lap YD</t>
   </si>
   <si>
-    <t>04.06.2020</t>
+    <t>01.12.2021</t>
+  </si>
+  <si>
+    <t>Зая</t>
+  </si>
+  <si>
+    <t>16.12.2018</t>
   </si>
   <si>
     <t>Жук</t>
-  </si>
-  <si>
-    <t>01.12.2021</t>
-  </si>
-  <si>
-    <t>Зая</t>
   </si>
 </sst>
 </file>
@@ -445,25 +472,54 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DAC3DF7-993F-4EC5-BDB7-B3E6620E5CBB}">
-  <dimension ref="A2:I9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CE212AB-0434-4F86-9898-2132FA0F1F69}">
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="E2">
         <v>123</v>
@@ -472,24 +528,24 @@
         <v>123</v>
       </c>
       <c r="G2" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="I2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="E3">
         <v>123</v>
@@ -498,27 +554,27 @@
         <v>123</v>
       </c>
       <c r="G3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="H3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="I3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="E4">
         <v>123</v>
@@ -527,27 +583,27 @@
         <v>123</v>
       </c>
       <c r="G4" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="H4" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="I4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1002</v>
       </c>
       <c r="B5" t="s">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="D5" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="E5">
         <v>123</v>
@@ -556,27 +612,27 @@
         <v>123</v>
       </c>
       <c r="G5" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="H5" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="I5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1003</v>
       </c>
       <c r="B6" t="s">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="C6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D6" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="E6">
         <v>123</v>
@@ -585,94 +641,94 @@
         <v>123</v>
       </c>
       <c r="G6" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="H6" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="I6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1004</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7">
+        <v>123</v>
+      </c>
+      <c r="F7">
+        <v>123</v>
+      </c>
+      <c r="G7" t="s">
+        <v>23</v>
+      </c>
+      <c r="H7" t="s">
+        <v>16</v>
+      </c>
+      <c r="I7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>2007</v>
+      </c>
+      <c r="B8" t="s">
         <v>9</v>
       </c>
-      <c r="D7" t="s">
-        <v>2</v>
-      </c>
-      <c r="E7">
-        <v>123</v>
-      </c>
-      <c r="F7">
-        <v>123</v>
-      </c>
-      <c r="G7" t="s">
+      <c r="C8" t="s">
         <v>14</v>
       </c>
-      <c r="H7" t="s">
-        <v>7</v>
-      </c>
-      <c r="I7" t="s">
+      <c r="D8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8" t="s">
+        <v>26</v>
+      </c>
+      <c r="I8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>3002</v>
+      </c>
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9">
         <v>15</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>2002</v>
-      </c>
-      <c r="B8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8">
-        <v>123</v>
-      </c>
-      <c r="F8">
-        <v>123</v>
-      </c>
-      <c r="G8" t="s">
-        <v>17</v>
-      </c>
-      <c r="I8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>2007</v>
-      </c>
-      <c r="B9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" t="s">
-        <v>1</v>
-      </c>
-      <c r="D9" t="s">
-        <v>18</v>
-      </c>
-      <c r="E9">
-        <v>1</v>
-      </c>
       <c r="F9">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="G9" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="I9" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>